<commit_message>
More Precise Distance with Vincenty's Formula
</commit_message>
<xml_diff>
--- a/Artillery/M795.xlsx
+++ b/Artillery/M795.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RStudio\MyProjects\Artillery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266344DF-FB80-4623-A8CC-08831955D206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415BA5AE-BD0C-479E-8CD9-7A20C6120A9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21735" yWindow="-3285" windowWidth="15375" windowHeight="7995" activeTab="1" xr2:uid="{ACD2B132-6E61-4758-88E4-4B02781318D4}"/>
+    <workbookView xWindow="20370" yWindow="-4845" windowWidth="29040" windowHeight="15990" xr2:uid="{ACD2B132-6E61-4758-88E4-4B02781318D4}"/>
   </bookViews>
   <sheets>
-    <sheet name="7R" sheetId="1" r:id="rId1"/>
-    <sheet name="4H" sheetId="2" r:id="rId2"/>
+    <sheet name="MACs" sheetId="3" r:id="rId1"/>
+    <sheet name="7R" sheetId="1" r:id="rId2"/>
+    <sheet name="4H" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>DFS</t>
   </si>
@@ -68,6 +69,33 @@
   </si>
   <si>
     <t>MaxOrd</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>M231 1L</t>
+  </si>
+  <si>
+    <t>Cas.p</t>
+  </si>
+  <si>
+    <t>Cas.n</t>
+  </si>
+  <si>
+    <t>Maxord.z</t>
+  </si>
+  <si>
+    <t>M231 2L</t>
+  </si>
+  <si>
+    <t>M232A1 3H</t>
+  </si>
+  <si>
+    <t>M232A1 4H</t>
+  </si>
+  <si>
+    <t>M232A1 5H</t>
   </si>
 </sst>
 </file>
@@ -123,6 +151,332 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MACs!$B$22:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MACs!$H$22:$H$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5232</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-21DE-4B94-B39F-D713500F45B1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="453896584"/>
+        <c:axId val="453895600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="453896584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="453895600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="453895600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="453896584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -602,6 +956,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1118,7 +1512,608 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571835</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>239</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55C72D9B-FF0B-419D-8962-4AEFB9C72922}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="571500"/>
+          <a:ext cx="2400635" cy="1714739"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B90ACD76-D898-4E77-931C-D6310E69A117}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1159,7 +2154,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1504,6 +2499,716 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C41F4F-EBAC-4919-9985-D9EB2643DC57}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2">
+        <v>61.9</v>
+      </c>
+      <c r="D2">
+        <v>3.6</v>
+      </c>
+      <c r="E2">
+        <v>1.2</v>
+      </c>
+      <c r="F2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G2">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="H2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <f>ROUND(AVERAGE(B4,B2),-3)</f>
+        <v>3000</v>
+      </c>
+      <c r="C3">
+        <v>201</v>
+      </c>
+      <c r="D3">
+        <v>11.3</v>
+      </c>
+      <c r="E3">
+        <v>3.9</v>
+      </c>
+      <c r="F3">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="G3">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="H3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <f>ROUND(AVERAGE(B6,B2),-3)</f>
+        <v>4000</v>
+      </c>
+      <c r="C4">
+        <v>282.7</v>
+      </c>
+      <c r="D4">
+        <v>15.7</v>
+      </c>
+      <c r="E4">
+        <v>5.7</v>
+      </c>
+      <c r="F4">
+        <v>0.09</v>
+      </c>
+      <c r="G4">
+        <v>-8.1000000000000003E-2</v>
+      </c>
+      <c r="H4">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <f>ROUND(AVERAGE(B6,B4),-3)</f>
+        <v>5000</v>
+      </c>
+      <c r="C5">
+        <v>379.1</v>
+      </c>
+      <c r="D5">
+        <v>20.7</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>0.193</v>
+      </c>
+      <c r="G5">
+        <v>-0.16800000000000001</v>
+      </c>
+      <c r="H5">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>6500</v>
+      </c>
+      <c r="C6">
+        <v>597.6</v>
+      </c>
+      <c r="D6">
+        <v>31.1</v>
+      </c>
+      <c r="E6">
+        <v>14.4</v>
+      </c>
+      <c r="F6">
+        <v>1.2589999999999999</v>
+      </c>
+      <c r="G6">
+        <v>-0.70099999999999996</v>
+      </c>
+      <c r="H6">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7">
+        <v>29.5</v>
+      </c>
+      <c r="D7">
+        <v>2.5</v>
+      </c>
+      <c r="E7">
+        <v>0.7</v>
+      </c>
+      <c r="F7">
+        <v>1E-3</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <f>ROUND(AVERAGE(B9,B7),-3)</f>
+        <v>4000</v>
+      </c>
+      <c r="C8">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="D8">
+        <v>11.3</v>
+      </c>
+      <c r="E8">
+        <v>3.3</v>
+      </c>
+      <c r="F8">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G8">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="H8">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <f>ROUND(AVERAGE(B11,B7),-3)</f>
+        <v>6000</v>
+      </c>
+      <c r="C9">
+        <v>246.4</v>
+      </c>
+      <c r="D9">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="E9">
+        <v>5.7</v>
+      </c>
+      <c r="F9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="G9">
+        <v>-3.4000000000000002E-2</v>
+      </c>
+      <c r="H9">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <f>ROUND(AVERAGE(B11,B9),-3)</f>
+        <v>8000</v>
+      </c>
+      <c r="C10">
+        <v>370.2</v>
+      </c>
+      <c r="D10">
+        <v>26.5</v>
+      </c>
+      <c r="E10">
+        <v>8.9</v>
+      </c>
+      <c r="F10">
+        <v>0.22</v>
+      </c>
+      <c r="G10">
+        <v>-0.17299999999999999</v>
+      </c>
+      <c r="H10">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>10500</v>
+      </c>
+      <c r="C11">
+        <v>603.4</v>
+      </c>
+      <c r="D11">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="E11">
+        <v>16.8</v>
+      </c>
+      <c r="F11">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="G11">
+        <v>-0.54</v>
+      </c>
+      <c r="H11">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+      <c r="C12">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D12">
+        <v>1.8</v>
+      </c>
+      <c r="E12">
+        <v>0.4</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <f>ROUND(AVERAGE(B14,B12),-3)</f>
+        <v>5000</v>
+      </c>
+      <c r="C13">
+        <v>106.3</v>
+      </c>
+      <c r="D13">
+        <v>11.1</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G13">
+        <v>-2E-3</v>
+      </c>
+      <c r="H13">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <f>ROUND(AVERAGE(B16,B12),-3)</f>
+        <v>8000</v>
+      </c>
+      <c r="C14">
+        <v>212.3</v>
+      </c>
+      <c r="D14">
+        <v>20.5</v>
+      </c>
+      <c r="E14">
+        <v>6.1</v>
+      </c>
+      <c r="F14">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="G14">
+        <v>-1.2999999999999999E-2</v>
+      </c>
+      <c r="H14">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <f>ROUND(AVERAGE(B16,B14),-3)</f>
+        <v>11000</v>
+      </c>
+      <c r="C15">
+        <v>360.1</v>
+      </c>
+      <c r="D15">
+        <v>31.9</v>
+      </c>
+      <c r="E15">
+        <v>10.7</v>
+      </c>
+      <c r="F15">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="G15">
+        <v>-6.4000000000000001E-2</v>
+      </c>
+      <c r="H15">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>14000</v>
+      </c>
+      <c r="C16">
+        <v>578.9</v>
+      </c>
+      <c r="D16">
+        <v>47.1</v>
+      </c>
+      <c r="E16">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="F16">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="G16">
+        <v>-0.35</v>
+      </c>
+      <c r="H16">
+        <v>2846</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>2000</v>
+      </c>
+      <c r="C17">
+        <v>23.7</v>
+      </c>
+      <c r="D17">
+        <v>3.2</v>
+      </c>
+      <c r="E17">
+        <v>0.7</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <f>ROUND(AVERAGE(B19,B17),-3)</f>
+        <v>6000</v>
+      </c>
+      <c r="C18">
+        <v>89.8</v>
+      </c>
+      <c r="D18">
+        <v>11.3</v>
+      </c>
+      <c r="E18">
+        <v>2.8</v>
+      </c>
+      <c r="F18">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G18">
+        <v>-1E-3</v>
+      </c>
+      <c r="H18">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <f>ROUND(AVERAGE(B21,B17),-3)</f>
+        <v>10000</v>
+      </c>
+      <c r="C19">
+        <v>197.7</v>
+      </c>
+      <c r="D19">
+        <v>22.7</v>
+      </c>
+      <c r="E19">
+        <v>6.4</v>
+      </c>
+      <c r="F19">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G19">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="H19">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f>ROUND(AVERAGE(B21,B19),-3)</f>
+        <v>14000</v>
+      </c>
+      <c r="C20">
+        <v>369.3</v>
+      </c>
+      <c r="D20">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E20">
+        <v>12.4</v>
+      </c>
+      <c r="F20">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G20">
+        <v>-5.5E-2</v>
+      </c>
+      <c r="H20">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>18000</v>
+      </c>
+      <c r="C21">
+        <v>668.1</v>
+      </c>
+      <c r="D21">
+        <v>60.2</v>
+      </c>
+      <c r="E21">
+        <v>25.4</v>
+      </c>
+      <c r="F21">
+        <v>1.589</v>
+      </c>
+      <c r="G21">
+        <v>-0.57699999999999996</v>
+      </c>
+      <c r="H21">
+        <v>4624</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>2000</v>
+      </c>
+      <c r="C22">
+        <v>17.5</v>
+      </c>
+      <c r="D22">
+        <v>2.7</v>
+      </c>
+      <c r="E22">
+        <v>0.8</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <f>ROUND(AVERAGE(B24,B22),-3)</f>
+        <v>7000</v>
+      </c>
+      <c r="C23">
+        <v>80.3</v>
+      </c>
+      <c r="D23">
+        <v>11.6</v>
+      </c>
+      <c r="E23">
+        <v>3.8</v>
+      </c>
+      <c r="F23">
+        <v>-1E-3</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <f>ROUND(AVERAGE(B26,B22),-3)</f>
+        <v>12000</v>
+      </c>
+      <c r="C24">
+        <v>190.7</v>
+      </c>
+      <c r="D24">
+        <v>24.8</v>
+      </c>
+      <c r="E24">
+        <v>8.5</v>
+      </c>
+      <c r="F24">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="G24">
+        <v>0.02</v>
+      </c>
+      <c r="H24">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <f>ROUND(AVERAGE(B26,B24),-3)</f>
+        <v>17000</v>
+      </c>
+      <c r="C25">
+        <v>377.5</v>
+      </c>
+      <c r="D25">
+        <v>43</v>
+      </c>
+      <c r="E25">
+        <v>14.9</v>
+      </c>
+      <c r="F25">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>2375</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26">
+        <v>21000</v>
+      </c>
+      <c r="C26">
+        <v>624.70000000000005</v>
+      </c>
+      <c r="D26">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="E26">
+        <v>22.9</v>
+      </c>
+      <c r="F26">
+        <v>0.5</v>
+      </c>
+      <c r="G26">
+        <v>-0.27800000000000002</v>
+      </c>
+      <c r="H26">
+        <v>5232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371A989B-35A3-421F-B767-FFBE138A6C5D}">
   <dimension ref="A1:I19"/>
   <sheetViews>
@@ -1815,11 +3520,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5777B8-458F-4FD1-BC5E-7D792F8D0E8B}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Getting ready to add grid declination to MGRS2UTM2LL from Desktop to git
</commit_message>
<xml_diff>
--- a/Artillery/M795.xlsx
+++ b/Artillery/M795.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RStudio\MyProjects\Artillery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415BA5AE-BD0C-479E-8CD9-7A20C6120A9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58463DC3-8422-4AB8-B659-AD79E7F5AA34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4845" windowWidth="29040" windowHeight="15990" xr2:uid="{ACD2B132-6E61-4758-88E4-4B02781318D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{ACD2B132-6E61-4758-88E4-4B02781318D4}"/>
   </bookViews>
   <sheets>
     <sheet name="MACs" sheetId="3" r:id="rId1"/>
@@ -237,9 +237,40 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -248,10 +279,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2000</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7000</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>12000</c:v>
@@ -267,7 +298,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MACs!$H$22:$H$26</c:f>
+              <c:f>MACs!$F$22:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -275,7 +306,7 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>163</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>760</c:v>
@@ -2032,16 +2063,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>571835</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>239</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95585</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95489</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2064,7 +2095,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6096000" y="571500"/>
+          <a:off x="5114925" y="1428750"/>
           <a:ext cx="2400635" cy="1714739"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2076,14 +2107,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
@@ -2503,7 +2534,8 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2528,13 +2560,13 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2542,25 +2574,25 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="C2">
-        <v>61.9</v>
+        <v>163.69999999999999</v>
       </c>
       <c r="D2">
-        <v>3.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E2">
-        <v>1.2</v>
+        <v>3.2</v>
       </c>
       <c r="F2">
-        <v>3.0000000000000001E-3</v>
+        <v>105</v>
       </c>
       <c r="G2">
-        <v>-3.0000000000000001E-3</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="H2">
-        <v>105</v>
+        <v>-2.4E-2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2569,25 +2601,25 @@
       </c>
       <c r="B3">
         <f>ROUND(AVERAGE(B4,B2),-3)</f>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="C3">
-        <v>201</v>
+        <v>282.5</v>
       </c>
       <c r="D3">
-        <v>11.3</v>
+        <v>15.7</v>
       </c>
       <c r="E3">
-        <v>3.9</v>
+        <v>5.7</v>
       </c>
       <c r="F3">
-        <v>4.1000000000000002E-2</v>
+        <v>301</v>
       </c>
       <c r="G3">
-        <v>-3.7999999999999999E-2</v>
+        <v>0.09</v>
       </c>
       <c r="H3">
-        <v>156</v>
+        <v>-8.1000000000000003E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2596,25 +2628,25 @@
       </c>
       <c r="B4">
         <f>ROUND(AVERAGE(B6,B2),-3)</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="C4">
-        <v>282.7</v>
+        <v>378.8</v>
       </c>
       <c r="D4">
-        <v>15.7</v>
+        <v>20.7</v>
       </c>
       <c r="E4">
-        <v>5.7</v>
+        <v>8</v>
       </c>
       <c r="F4">
-        <v>0.09</v>
+        <v>521</v>
       </c>
       <c r="G4">
-        <v>-8.1000000000000003E-2</v>
+        <v>0.193</v>
       </c>
       <c r="H4">
-        <v>301</v>
+        <v>-0.16800000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2623,25 +2655,25 @@
       </c>
       <c r="B5">
         <f>ROUND(AVERAGE(B6,B4),-3)</f>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="C5">
-        <v>379.1</v>
+        <v>504.8</v>
       </c>
       <c r="D5">
-        <v>20.7</v>
+        <v>26.9</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>0.193</v>
+        <v>878</v>
       </c>
       <c r="G5">
-        <v>-0.16800000000000001</v>
+        <v>0.498</v>
       </c>
       <c r="H5">
-        <v>521</v>
+        <v>-0.38300000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2652,22 +2684,22 @@
         <v>6500</v>
       </c>
       <c r="C6">
-        <v>597.6</v>
+        <v>596.79999999999995</v>
       </c>
       <c r="D6">
         <v>31.1</v>
       </c>
       <c r="E6">
-        <v>14.4</v>
+        <v>16</v>
       </c>
       <c r="F6">
+        <v>1175</v>
+      </c>
+      <c r="G6">
         <v>1.2589999999999999</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>-0.70099999999999996</v>
-      </c>
-      <c r="H6">
-        <v>1175</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2675,25 +2707,25 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="C7">
-        <v>29.5</v>
+        <v>101.7</v>
       </c>
       <c r="D7">
-        <v>2.5</v>
+        <v>8.1</v>
       </c>
       <c r="E7">
-        <v>0.7</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>1E-3</v>
+        <v>83</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H7">
-        <v>83</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2702,25 +2734,25 @@
       </c>
       <c r="B8">
         <f>ROUND(AVERAGE(B9,B7),-3)</f>
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="C8">
-        <v>145.19999999999999</v>
+        <v>193.2</v>
       </c>
       <c r="D8">
-        <v>11.3</v>
+        <v>14.8</v>
       </c>
       <c r="E8">
-        <v>3.3</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>1.4E-2</v>
+        <v>274</v>
       </c>
       <c r="G8">
-        <v>-1.0999999999999999E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="H8">
-        <v>161</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2729,25 +2761,25 @@
       </c>
       <c r="B9">
         <f>ROUND(AVERAGE(B11,B7),-3)</f>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="C9">
-        <v>246.4</v>
+        <v>304.60000000000002</v>
       </c>
       <c r="D9">
-        <v>18.399999999999999</v>
+        <v>22.3</v>
       </c>
       <c r="E9">
-        <v>5.7</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>4.1000000000000002E-2</v>
+        <v>626</v>
       </c>
       <c r="G9">
-        <v>-3.4000000000000002E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="H9">
-        <v>426</v>
+        <v>-5.7000000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2756,25 +2788,25 @@
       </c>
       <c r="B10">
         <f>ROUND(AVERAGE(B11,B9),-3)</f>
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="C10">
-        <v>370.2</v>
+        <v>445.8</v>
       </c>
       <c r="D10">
-        <v>26.5</v>
+        <v>31.3</v>
       </c>
       <c r="E10">
-        <v>8.9</v>
+        <v>12</v>
       </c>
       <c r="F10">
+        <v>1226</v>
+      </c>
+      <c r="G10">
         <v>0.22</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>-0.17299999999999999</v>
-      </c>
-      <c r="H10">
-        <v>884</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2785,22 +2817,22 @@
         <v>10500</v>
       </c>
       <c r="C11">
-        <v>603.4</v>
+        <v>602.9</v>
       </c>
       <c r="D11">
         <v>40.700000000000003</v>
       </c>
       <c r="E11">
-        <v>16.8</v>
+        <v>18</v>
       </c>
       <c r="F11">
+        <v>2053</v>
+      </c>
+      <c r="G11">
         <v>0.95899999999999996</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>-0.54</v>
-      </c>
-      <c r="H11">
-        <v>2053</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2808,25 +2840,25 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="C12">
-        <v>16.399999999999999</v>
+        <v>55.5</v>
       </c>
       <c r="D12">
-        <v>1.8</v>
+        <v>6</v>
       </c>
       <c r="E12">
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="H12">
-        <v>45</v>
+        <v>-1E-3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2835,25 +2867,25 @@
       </c>
       <c r="B13">
         <f>ROUND(AVERAGE(B14,B12),-3)</f>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="C13">
-        <v>106.3</v>
+        <v>136.9</v>
       </c>
       <c r="D13">
-        <v>11.1</v>
+        <v>13.5</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>4.7</v>
       </c>
       <c r="F13">
-        <v>5.0000000000000001E-3</v>
+        <v>242</v>
       </c>
       <c r="G13">
-        <v>-2E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H13">
-        <v>151</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2862,25 +2894,25 @@
       </c>
       <c r="B14">
         <f>ROUND(AVERAGE(B16,B12),-3)</f>
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="C14">
-        <v>212.3</v>
+        <v>256.10000000000002</v>
       </c>
       <c r="D14">
-        <v>20.5</v>
+        <v>24</v>
       </c>
       <c r="E14">
-        <v>6.1</v>
+        <v>7.8</v>
       </c>
       <c r="F14">
-        <v>2.1999999999999999E-2</v>
+        <v>736</v>
       </c>
       <c r="G14">
-        <v>-1.2999999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="H14">
-        <v>529</v>
+        <v>-2.3E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2889,25 +2921,25 @@
       </c>
       <c r="B15">
         <f>ROUND(AVERAGE(B16,B14),-3)</f>
-        <v>11000</v>
+        <v>12000</v>
       </c>
       <c r="C15">
-        <v>360.1</v>
+        <v>420.5</v>
       </c>
       <c r="D15">
-        <v>31.9</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="E15">
-        <v>10.7</v>
+        <v>13.4</v>
       </c>
       <c r="F15">
-        <v>8.6999999999999994E-2</v>
+        <v>1702</v>
       </c>
       <c r="G15">
-        <v>-6.4000000000000001E-2</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="H15">
-        <v>1312</v>
+        <v>-0.105</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2918,22 +2950,22 @@
         <v>14000</v>
       </c>
       <c r="C16">
-        <v>578.9</v>
+        <v>577.70000000000005</v>
       </c>
       <c r="D16">
         <v>47.1</v>
       </c>
       <c r="E16">
-        <v>18.899999999999999</v>
+        <v>20</v>
       </c>
       <c r="F16">
+        <v>2846</v>
+      </c>
+      <c r="G16">
         <v>0.54800000000000004</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>-0.35</v>
-      </c>
-      <c r="H16">
-        <v>2846</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2941,25 +2973,25 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="C17">
-        <v>23.7</v>
+        <v>37.5</v>
       </c>
       <c r="D17">
-        <v>3.2</v>
+        <v>4.5</v>
       </c>
       <c r="E17">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F17">
+        <v>30</v>
+      </c>
+      <c r="G17">
+        <v>1E-3</v>
+      </c>
+      <c r="H17">
         <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2968,25 +3000,25 @@
       </c>
       <c r="B18">
         <f>ROUND(AVERAGE(B19,B17),-3)</f>
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="C18">
-        <v>89.8</v>
+        <v>111.6</v>
       </c>
       <c r="D18">
-        <v>11.3</v>
+        <v>13.7</v>
       </c>
       <c r="E18">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="F18">
-        <v>3.0000000000000001E-3</v>
+        <v>231</v>
       </c>
       <c r="G18">
-        <v>-1E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H18">
-        <v>154</v>
+        <v>-2E-3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2995,25 +3027,25 @@
       </c>
       <c r="B19">
         <f>ROUND(AVERAGE(B21,B17),-3)</f>
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="C19">
-        <v>197.7</v>
+        <v>233.5</v>
       </c>
       <c r="D19">
-        <v>22.7</v>
+        <v>26.1</v>
       </c>
       <c r="E19">
-        <v>6.4</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="F19">
-        <v>1.4999999999999999E-2</v>
+        <v>851</v>
       </c>
       <c r="G19">
-        <v>-5.0000000000000001E-3</v>
+        <v>2.3E-2</v>
       </c>
       <c r="H19">
-        <v>637</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3022,25 +3054,25 @@
       </c>
       <c r="B20">
         <f>ROUND(AVERAGE(B21,B19),-3)</f>
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="C20">
-        <v>369.3</v>
+        <v>424.4</v>
       </c>
       <c r="D20">
-        <v>37.700000000000003</v>
+        <v>42.1</v>
       </c>
       <c r="E20">
-        <v>12.4</v>
+        <v>15.3</v>
       </c>
       <c r="F20">
-        <v>8.4000000000000005E-2</v>
+        <v>2291</v>
       </c>
       <c r="G20">
-        <v>-5.5E-2</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="H20">
-        <v>1823</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3051,22 +3083,22 @@
         <v>18000</v>
       </c>
       <c r="C21">
-        <v>668.1</v>
+        <v>666.5</v>
       </c>
       <c r="D21">
         <v>60.2</v>
       </c>
       <c r="E21">
-        <v>25.4</v>
+        <v>26.4</v>
       </c>
       <c r="F21">
+        <v>4624</v>
+      </c>
+      <c r="G21">
         <v>1.589</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>-0.57699999999999996</v>
-      </c>
-      <c r="H21">
-        <v>4624</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -3074,25 +3106,25 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="C22">
-        <v>17.5</v>
+        <v>27.5</v>
       </c>
       <c r="D22">
-        <v>2.7</v>
+        <v>4.2</v>
       </c>
       <c r="E22">
-        <v>0.8</v>
+        <v>1.3</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3101,25 +3133,25 @@
       </c>
       <c r="B23">
         <f>ROUND(AVERAGE(B24,B22),-3)</f>
-        <v>7000</v>
+        <v>8000</v>
       </c>
       <c r="C23">
-        <v>80.3</v>
+        <v>97.2</v>
       </c>
       <c r="D23">
-        <v>11.6</v>
+        <v>13.4</v>
       </c>
       <c r="E23">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
       <c r="F23">
-        <v>-1E-3</v>
+        <v>233</v>
       </c>
       <c r="G23">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="H23">
         <v>0</v>
-      </c>
-      <c r="H23">
-        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3131,22 +3163,22 @@
         <v>12000</v>
       </c>
       <c r="C24">
-        <v>190.7</v>
+        <v>190.3</v>
       </c>
       <c r="D24">
-        <v>24.8</v>
+        <v>24.4</v>
       </c>
       <c r="E24">
-        <v>8.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="F24">
+        <v>760</v>
+      </c>
+      <c r="G24">
         <v>-1.2E-2</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>0.02</v>
-      </c>
-      <c r="H24">
-        <v>760</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3161,19 +3193,19 @@
         <v>377.5</v>
       </c>
       <c r="D25">
-        <v>43</v>
+        <v>42.5</v>
       </c>
       <c r="E25">
-        <v>14.9</v>
+        <v>16</v>
       </c>
       <c r="F25">
+        <v>2375</v>
+      </c>
+      <c r="G25">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>0</v>
-      </c>
-      <c r="H25">
-        <v>2375</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3184,22 +3216,22 @@
         <v>21000</v>
       </c>
       <c r="C26">
-        <v>624.70000000000005</v>
+        <v>623.6</v>
       </c>
       <c r="D26">
         <v>64.099999999999994</v>
       </c>
       <c r="E26">
-        <v>22.9</v>
+        <v>24</v>
       </c>
       <c r="F26">
+        <v>5232</v>
+      </c>
+      <c r="G26">
         <v>0.5</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>-0.27800000000000002</v>
-      </c>
-      <c r="H26">
-        <v>5232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added corrected range; More accurate CSF; Made the trajectory more pretty.
</commit_message>
<xml_diff>
--- a/Artillery/M795.xlsx
+++ b/Artillery/M795.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RStudio\MyProjects\Artillery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58463DC3-8422-4AB8-B659-AD79E7F5AA34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82C4FF6-4C9E-4BF1-AE3C-482CFD5E1A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{ACD2B132-6E61-4758-88E4-4B02781318D4}"/>
   </bookViews>
   <sheets>
     <sheet name="MACs" sheetId="3" r:id="rId1"/>
-    <sheet name="7R" sheetId="1" r:id="rId2"/>
-    <sheet name="4H" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="7R" sheetId="1" r:id="rId3"/>
+    <sheet name="4H" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
   <si>
     <t>DFS</t>
   </si>
@@ -96,6 +97,24 @@
   </si>
   <si>
     <t>M232A1 5H</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>QE 10%VI</t>
+  </si>
+  <si>
+    <t>AOS</t>
+  </si>
+  <si>
+    <t>QE -10%VI</t>
+  </si>
+  <si>
+    <t>tCas.p</t>
+  </si>
+  <si>
+    <t>tCas.n</t>
   </si>
 </sst>
 </file>
@@ -227,95 +246,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="6"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="0"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>MACs!$B$22:$B$26</c:f>
+              <c:f>MACs!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3000</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8000</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>12000</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17000</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21000</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>MACs!$F$22:$F$26</c:f>
+              <c:f>MACs!$I$2:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>2.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>233</c:v>
+                  <c:v>4.1000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>760</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2375</c:v>
+                  <c:v>0.193</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5232</c:v>
+                  <c:v>0.498</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2063,16 +2037,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>95585</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95489</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>571835</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>162164</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2095,7 +2069,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5114925" y="1428750"/>
+          <a:off x="11077575" y="161925"/>
           <a:ext cx="2400635" cy="1714739"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2107,16 +2081,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2531,11 +2505,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C41F4F-EBAC-4919-9985-D9EB2643DC57}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,7 +2517,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2568,8 +2542,32 @@
       <c r="H1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2580,129 +2578,276 @@
         <v>163.69999999999999</v>
       </c>
       <c r="D2">
-        <v>9.3000000000000007</v>
+        <v>9</v>
       </c>
       <c r="E2">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="F2">
         <v>105</v>
       </c>
       <c r="G2">
+        <f>(N2-L2)/ABS(L2)</f>
+        <v>2.4411975979328097E-2</v>
+      </c>
+      <c r="H2">
+        <f>(Q2-O2)/ABS(O2)</f>
+        <v>-2.4411975979327954E-2</v>
+      </c>
+      <c r="I2">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>-2.4E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>ATAN(400/4000)*3200/PI()</f>
+        <v>101.52165577777143</v>
+      </c>
+      <c r="M2">
+        <v>267.7</v>
+      </c>
+      <c r="N2">
+        <f>M2-C2</f>
+        <v>104</v>
+      </c>
+      <c r="O2">
+        <f>ATAN(-400/4000)*3200/PI()</f>
+        <v>-101.52165577777143</v>
+      </c>
+      <c r="P2">
+        <v>59.7</v>
+      </c>
+      <c r="Q2">
+        <f>P2-C2</f>
+        <v>-103.99999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3">
-        <f>ROUND(AVERAGE(B4,B2),-3)</f>
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="C3">
-        <v>282.5</v>
+        <v>197.8</v>
       </c>
       <c r="D3">
-        <v>15.7</v>
+        <v>11</v>
       </c>
       <c r="E3">
-        <v>5.7</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>301</v>
+        <v>153</v>
       </c>
       <c r="G3">
-        <v>0.09</v>
+        <f>(N3-L3)/ABS(L3)</f>
+        <v>4.1157171740528541E-2</v>
       </c>
       <c r="H3">
-        <v>-8.1000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <f>(Q3-O3)/ABS(O3)</f>
+        <v>-3.3277079617610797E-2</v>
+      </c>
+      <c r="I3">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="J3">
+        <v>-3.7999999999999999E-2</v>
+      </c>
+      <c r="L3">
+        <f>ATAN(400/4000)*3200/PI()</f>
+        <v>101.52165577777143</v>
+      </c>
+      <c r="M3">
+        <v>303.5</v>
+      </c>
+      <c r="N3">
+        <f>M3-C3</f>
+        <v>105.69999999999999</v>
+      </c>
+      <c r="O3">
+        <f>ATAN(-400/4000)*3200/PI()</f>
+        <v>-101.52165577777143</v>
+      </c>
+      <c r="P3">
+        <v>92.9</v>
+      </c>
+      <c r="Q3">
+        <f>P3-C3</f>
+        <v>-104.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4">
-        <f>ROUND(AVERAGE(B6,B2),-3)</f>
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="C4">
-        <v>378.8</v>
+        <v>282.60000000000002</v>
       </c>
       <c r="D4">
-        <v>20.7</v>
+        <v>15</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>521</v>
+        <v>301</v>
       </c>
       <c r="G4">
-        <v>0.193</v>
+        <f>(N4-L4)/ABS(L4)</f>
+        <v>9.43477935702242E-2</v>
       </c>
       <c r="H4">
-        <v>-0.16800000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f>(Q4-O4)/ABS(O4)</f>
+        <v>-7.957262083975368E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.09</v>
+      </c>
+      <c r="J4">
+        <v>-8.1000000000000003E-2</v>
+      </c>
+      <c r="L4">
+        <f>ATAN(400/4000)*3200/PI()</f>
+        <v>101.52165577777143</v>
+      </c>
+      <c r="M4">
+        <v>393.7</v>
+      </c>
+      <c r="N4">
+        <f>M4-C4</f>
+        <v>111.09999999999997</v>
+      </c>
+      <c r="O4">
+        <f>ATAN(-400/4000)*3200/PI()</f>
+        <v>-101.52165577777143</v>
+      </c>
+      <c r="P4">
+        <v>173</v>
+      </c>
+      <c r="Q4">
+        <f>P4-C4</f>
+        <v>-109.60000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5">
-        <f>ROUND(AVERAGE(B6,B4),-3)</f>
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="C5">
-        <v>504.8</v>
+        <v>378.8</v>
       </c>
       <c r="D5">
-        <v>26.9</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>878</v>
+        <v>521</v>
       </c>
       <c r="G5">
-        <v>0.498</v>
+        <f>(N5-L5)/ABS(L5)</f>
+        <v>0.20762411783716914</v>
       </c>
       <c r="H5">
-        <v>-0.38300000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <f>(Q5-O5)/ABS(O5)</f>
+        <v>-0.15935855358429715</v>
+      </c>
+      <c r="I5">
+        <v>0.193</v>
+      </c>
+      <c r="J5">
+        <v>-0.16800000000000001</v>
+      </c>
+      <c r="L5">
+        <f>ATAN(400/4000)*3200/PI()</f>
+        <v>101.52165577777143</v>
+      </c>
+      <c r="M5">
+        <v>501.4</v>
+      </c>
+      <c r="N5">
+        <f>M5-C5</f>
+        <v>122.59999999999997</v>
+      </c>
+      <c r="O5">
+        <f>ATAN(-400/4000)*3200/PI()</f>
+        <v>-101.52165577777143</v>
+      </c>
+      <c r="P5">
+        <v>261.10000000000002</v>
+      </c>
+      <c r="Q5">
+        <f>P5-C5</f>
+        <v>-117.69999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
-        <v>6500</v>
+        <v>6000</v>
       </c>
       <c r="C6">
-        <v>596.79999999999995</v>
+        <v>481.2</v>
       </c>
       <c r="D6">
-        <v>31.1</v>
+        <v>25</v>
       </c>
       <c r="E6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F6">
-        <v>1175</v>
+        <v>818</v>
       </c>
       <c r="G6">
-        <v>1.2589999999999999</v>
+        <f>(N6-L6)/ABS(L6)</f>
+        <v>0.47456223850101348</v>
       </c>
       <c r="H6">
-        <v>-0.70099999999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <f>(Q6-O6)/ABS(O6)</f>
+        <v>-0.29627515421999562</v>
+      </c>
+      <c r="I6">
+        <v>0.498</v>
+      </c>
+      <c r="J6">
+        <v>-3.83</v>
+      </c>
+      <c r="L6">
+        <f>ATAN(400/4000)*3200/PI()</f>
+        <v>101.52165577777143</v>
+      </c>
+      <c r="M6">
+        <v>630.9</v>
+      </c>
+      <c r="N6">
+        <f>M6-C6</f>
+        <v>149.69999999999999</v>
+      </c>
+      <c r="O6">
+        <f>ATAN(-400/4000)*3200/PI()</f>
+        <v>-101.52165577777143</v>
+      </c>
+      <c r="P6">
+        <v>349.6</v>
+      </c>
+      <c r="Q6">
+        <f>P6-C6</f>
+        <v>-131.59999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2721,516 +2866,644 @@
       <c r="F7">
         <v>83</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8">
-        <f>ROUND(AVERAGE(B9,B7),-3)</f>
-        <v>5000</v>
-      </c>
-      <c r="C8">
-        <v>193.2</v>
-      </c>
-      <c r="D8">
-        <v>14.8</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>274</v>
-      </c>
-      <c r="G8">
-        <v>2.4E-2</v>
-      </c>
-      <c r="H8">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9">
         <f>ROUND(AVERAGE(B11,B7),-3)</f>
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="C9">
-        <v>304.60000000000002</v>
+        <v>193.2</v>
       </c>
       <c r="D9">
-        <v>22.3</v>
+        <v>14.8</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F9">
-        <v>626</v>
-      </c>
-      <c r="G9">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="H9">
-        <v>-5.7000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+      <c r="I9">
+        <v>2.4E-2</v>
+      </c>
+      <c r="J9">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10">
-        <f>ROUND(AVERAGE(B11,B9),-3)</f>
-        <v>9000</v>
-      </c>
-      <c r="C10">
-        <v>445.8</v>
-      </c>
-      <c r="D10">
-        <v>31.3</v>
-      </c>
-      <c r="E10">
-        <v>12</v>
-      </c>
-      <c r="F10">
-        <v>1226</v>
-      </c>
-      <c r="G10">
-        <v>0.22</v>
-      </c>
-      <c r="H10">
-        <v>-0.17299999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11">
+        <f>ROUND(AVERAGE(B15,B7),-3)</f>
+        <v>7000</v>
+      </c>
+      <c r="C11">
+        <v>304.60000000000002</v>
+      </c>
+      <c r="D11">
+        <v>22.3</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>626</v>
+      </c>
+      <c r="I11">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="J11">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <f>ROUND(AVERAGE(B15,B11),-3)</f>
+        <v>9000</v>
+      </c>
+      <c r="C13">
+        <v>445.8</v>
+      </c>
+      <c r="D13">
+        <v>31.3</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>1226</v>
+      </c>
+      <c r="I13">
+        <v>0.22</v>
+      </c>
+      <c r="J13">
+        <v>-0.17299999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
         <v>10500</v>
       </c>
-      <c r="C11">
+      <c r="C15">
         <v>602.9</v>
       </c>
-      <c r="D11">
+      <c r="D15">
         <v>40.700000000000003</v>
       </c>
-      <c r="E11">
+      <c r="E15">
         <v>18</v>
       </c>
-      <c r="F11">
+      <c r="F15">
         <v>2053</v>
       </c>
-      <c r="G11">
+      <c r="I15">
         <v>0.95899999999999996</v>
       </c>
-      <c r="H11">
+      <c r="J15">
         <v>-0.54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <v>3000</v>
-      </c>
-      <c r="C12">
-        <v>55.5</v>
-      </c>
-      <c r="D12">
-        <v>6</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>45</v>
-      </c>
-      <c r="G12">
-        <v>1E-3</v>
-      </c>
-      <c r="H12">
-        <v>-1E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <f>ROUND(AVERAGE(B14,B12),-3)</f>
-        <v>6000</v>
-      </c>
-      <c r="C13">
-        <v>136.9</v>
-      </c>
-      <c r="D13">
-        <v>13.5</v>
-      </c>
-      <c r="E13">
-        <v>4.7</v>
-      </c>
-      <c r="F13">
-        <v>242</v>
-      </c>
-      <c r="G13">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="H13">
-        <v>-4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <f>ROUND(AVERAGE(B16,B12),-3)</f>
-        <v>9000</v>
-      </c>
-      <c r="C14">
-        <v>256.10000000000002</v>
-      </c>
-      <c r="D14">
-        <v>24</v>
-      </c>
-      <c r="E14">
-        <v>7.8</v>
-      </c>
-      <c r="F14">
-        <v>736</v>
-      </c>
-      <c r="G14">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="H14">
-        <v>-2.3E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <f>ROUND(AVERAGE(B16,B14),-3)</f>
-        <v>12000</v>
-      </c>
-      <c r="C15">
-        <v>420.5</v>
-      </c>
-      <c r="D15">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="E15">
-        <v>13.4</v>
-      </c>
-      <c r="F15">
-        <v>1702</v>
-      </c>
-      <c r="G15">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="H15">
-        <v>-0.105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16">
+        <v>3000</v>
+      </c>
+      <c r="C16">
+        <v>55.5</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>45</v>
+      </c>
+      <c r="I16">
+        <v>1E-3</v>
+      </c>
+      <c r="J16">
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <f>ROUND(AVERAGE(B20,B16),-3)</f>
+        <v>6000</v>
+      </c>
+      <c r="C18">
+        <v>136.9</v>
+      </c>
+      <c r="D18">
+        <v>13.5</v>
+      </c>
+      <c r="E18">
+        <v>4.7</v>
+      </c>
+      <c r="F18">
+        <v>242</v>
+      </c>
+      <c r="I18">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J18">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f>ROUND(AVERAGE(B24,B16),-3)</f>
+        <v>9000</v>
+      </c>
+      <c r="C20">
+        <v>256.10000000000002</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+      <c r="E20">
+        <v>7.8</v>
+      </c>
+      <c r="F20">
+        <v>736</v>
+      </c>
+      <c r="I20">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="J20">
+        <v>-2.3E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <f>ROUND(AVERAGE(B24,B20),-3)</f>
+        <v>12000</v>
+      </c>
+      <c r="C22">
+        <v>420.5</v>
+      </c>
+      <c r="D22">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E22">
+        <v>13.4</v>
+      </c>
+      <c r="F22">
+        <v>1702</v>
+      </c>
+      <c r="I22">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="J22">
+        <v>-0.105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24">
         <v>14000</v>
       </c>
-      <c r="C16">
+      <c r="C24">
         <v>577.70000000000005</v>
       </c>
-      <c r="D16">
+      <c r="D24">
         <v>47.1</v>
       </c>
-      <c r="E16">
+      <c r="E24">
         <v>20</v>
       </c>
-      <c r="F16">
+      <c r="F24">
         <v>2846</v>
       </c>
-      <c r="G16">
+      <c r="I24">
         <v>0.54800000000000004</v>
       </c>
-      <c r="H16">
+      <c r="J24">
         <v>-0.35</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
+      <c r="B25">
         <v>3000</v>
       </c>
-      <c r="C17">
+      <c r="C25">
         <v>37.5</v>
       </c>
-      <c r="D17">
+      <c r="D25">
         <v>4.5</v>
       </c>
-      <c r="E17">
+      <c r="E25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F17">
+      <c r="F25">
         <v>30</v>
       </c>
-      <c r="G17">
+      <c r="I25">
         <v>1E-3</v>
       </c>
-      <c r="H17">
+      <c r="J25">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
-        <f>ROUND(AVERAGE(B19,B17),-3)</f>
+      <c r="B26">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <f>ROUND(AVERAGE(B29,B25),-3)</f>
         <v>7000</v>
       </c>
-      <c r="C18">
+      <c r="C27">
         <v>111.6</v>
       </c>
-      <c r="D18">
+      <c r="D27">
         <v>13.7</v>
       </c>
-      <c r="E18">
+      <c r="E27">
         <v>3.5</v>
       </c>
-      <c r="F18">
+      <c r="F27">
         <v>231</v>
       </c>
-      <c r="G18">
+      <c r="I27">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H18">
+      <c r="J27">
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
-        <f>ROUND(AVERAGE(B21,B17),-3)</f>
+      <c r="B28">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <f>ROUND(AVERAGE(B33,B25),-3)</f>
         <v>11000</v>
       </c>
-      <c r="C19">
+      <c r="C29">
         <v>233.5</v>
       </c>
-      <c r="D19">
+      <c r="D29">
         <v>26.1</v>
       </c>
-      <c r="E19">
+      <c r="E29">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F19">
+      <c r="F29">
         <v>851</v>
       </c>
-      <c r="G19">
+      <c r="I29">
         <v>2.3E-2</v>
       </c>
-      <c r="H19">
+      <c r="J29">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
-        <f>ROUND(AVERAGE(B21,B19),-3)</f>
+      <c r="B30">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31">
+        <f>ROUND(AVERAGE(B33,B29),-3)</f>
         <v>15000</v>
       </c>
-      <c r="C20">
+      <c r="C31">
         <v>424.4</v>
       </c>
-      <c r="D20">
+      <c r="D31">
         <v>42.1</v>
       </c>
-      <c r="E20">
+      <c r="E31">
         <v>15.3</v>
       </c>
-      <c r="F20">
+      <c r="F31">
         <v>2291</v>
       </c>
-      <c r="G20">
+      <c r="I31">
         <v>0.13100000000000001</v>
       </c>
-      <c r="H20">
+      <c r="J31">
         <v>-0.09</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B32">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
         <v>18000</v>
       </c>
-      <c r="C21">
+      <c r="C33">
         <v>666.5</v>
       </c>
-      <c r="D21">
+      <c r="D33">
         <v>60.2</v>
       </c>
-      <c r="E21">
+      <c r="E33">
         <v>26.4</v>
       </c>
-      <c r="F21">
+      <c r="F33">
         <v>4624</v>
       </c>
-      <c r="G21">
+      <c r="I33">
         <v>1.589</v>
       </c>
-      <c r="H21">
+      <c r="J33">
         <v>-0.57699999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B34">
         <v>3000</v>
       </c>
-      <c r="C22">
+      <c r="C34">
         <v>27.5</v>
       </c>
-      <c r="D22">
+      <c r="D34">
         <v>4.2</v>
       </c>
-      <c r="E22">
+      <c r="E34">
         <v>1.3</v>
       </c>
-      <c r="F22">
+      <c r="F34">
         <v>22</v>
       </c>
-      <c r="G22">
+      <c r="I34">
         <v>0</v>
       </c>
-      <c r="H22">
+      <c r="J34">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>20</v>
       </c>
-      <c r="B23">
-        <f>ROUND(AVERAGE(B24,B22),-3)</f>
+      <c r="B35">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <f>ROUND(AVERAGE(B38,B34),-3)</f>
         <v>8000</v>
       </c>
-      <c r="C23">
+      <c r="C36">
         <v>97.2</v>
       </c>
-      <c r="D23">
+      <c r="D36">
         <v>13.4</v>
       </c>
-      <c r="E23">
+      <c r="E36">
         <v>4.8</v>
       </c>
-      <c r="F23">
+      <c r="F36">
         <v>233</v>
       </c>
-      <c r="G23">
+      <c r="I36">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="H23">
+      <c r="J36">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>20</v>
       </c>
-      <c r="B24">
-        <f>ROUND(AVERAGE(B26,B22),-3)</f>
+      <c r="B37">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38">
+        <f>ROUND(AVERAGE(B42,B34),-3)</f>
         <v>12000</v>
       </c>
-      <c r="C24">
+      <c r="C38">
         <v>190.3</v>
       </c>
-      <c r="D24">
+      <c r="D38">
         <v>24.4</v>
       </c>
-      <c r="E24">
+      <c r="E38">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F24">
+      <c r="F38">
         <v>760</v>
       </c>
-      <c r="G24">
+      <c r="I38">
         <v>-1.2E-2</v>
       </c>
-      <c r="H24">
+      <c r="J38">
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>20</v>
       </c>
-      <c r="B25">
-        <f>ROUND(AVERAGE(B26,B24),-3)</f>
+      <c r="B39">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <f>ROUND(AVERAGE(B42,B38),-3)</f>
         <v>17000</v>
       </c>
-      <c r="C25">
+      <c r="C40">
         <v>377.5</v>
       </c>
-      <c r="D25">
+      <c r="D40">
         <v>42.5</v>
       </c>
-      <c r="E25">
+      <c r="E40">
         <v>16</v>
       </c>
-      <c r="F25">
+      <c r="F40">
         <v>2375</v>
       </c>
-      <c r="G25">
+      <c r="I40">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H25">
+      <c r="J40">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>20</v>
       </c>
-      <c r="B26">
+      <c r="B41">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42">
         <v>21000</v>
       </c>
-      <c r="C26">
+      <c r="C42">
         <v>623.6</v>
       </c>
-      <c r="D26">
+      <c r="D42">
         <v>64.099999999999994</v>
       </c>
-      <c r="E26">
+      <c r="E42">
         <v>24</v>
       </c>
-      <c r="F26">
+      <c r="F42">
         <v>5232</v>
       </c>
-      <c r="G26">
+      <c r="I42">
         <v>0.5</v>
       </c>
-      <c r="H26">
+      <c r="J42">
         <v>-0.27800000000000002</v>
       </c>
     </row>
@@ -3241,6 +3514,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4670200D-FCB4-4365-B586-1F17B816050D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371A989B-35A3-421F-B767-FFBE138A6C5D}">
   <dimension ref="A1:I19"/>
   <sheetViews>
@@ -3552,7 +3837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5777B8-458F-4FD1-BC5E-7D792F8D0E8B}">
   <dimension ref="A1:E8"/>
   <sheetViews>

</xml_diff>